<commit_message>
updated background and  a lot of features
</commit_message>
<xml_diff>
--- a/new_templates/Water_Balance_TimeSeries_Template_v2.xlsx
+++ b/new_templates/Water_Balance_TimeSeries_Template_v2.xlsx
@@ -3,18 +3,18 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3588" yWindow="960" windowWidth="17280" windowHeight="8880" tabRatio="600" firstSheet="6" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3588" yWindow="960" windowWidth="17280" windowHeight="8880" tabRatio="600" firstSheet="6" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Reference Guide" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Flows_NEWTSF" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Flows_OLDTSF" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Flows_UG2P" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Flows_UG2S" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Flows_UG2N" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Flows_MERP" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Flows_MERS" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="Flows_STOCKPILE" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Flows_New TSF" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Flows_Old TSF" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Flows_UG2 Plant" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Flows_UG2 Main" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Flows_UG2 North" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Flows_Merensky Plant" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Flows_Merensky South" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Flows_Stockpile1" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>

</xml_diff>